<commit_message>
weekend will come again
</commit_message>
<xml_diff>
--- a/namesToRemember.xlsx
+++ b/namesToRemember.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\markdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06F4BEC0-D167-4963-B6F7-1D778C978C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93153E6E-E580-4623-9F98-6545A5E3768D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="16365" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11955" yWindow="315" windowWidth="16365" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>gantt chart</t>
+  </si>
+  <si>
+    <t>Kerckhoff</t>
+  </si>
+  <si>
+    <t>Kerckhoffs’ Prinzip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Kerckhoffs’sche Prinzip oder Kerckhoffs’ Maxime ist ein im Jahr 1883 von Auguste Kerckhoffs formulierter Grundsatz der modernen Kryptographie, welcher besagt, dass die Sicherheit eines (symmetrischen) Verschlüsselungsverfahrens auf der Geheimhaltung des Schlüssels beruht anstatt auf der Geheimhaltung des Verschlüsselungsalgorithmus. </t>
   </si>
 </sst>
 </file>
@@ -491,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32.25" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -583,12 +592,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="105.75" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>